<commit_message>
Log In functionality is ready (hope). For some reason the LogIn button isn't pressed as expected
</commit_message>
<xml_diff>
--- a/Tests/Data/DataSource.xlsx
+++ b/Tests/Data/DataSource.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\GitHub\QA-Automation-Teamwork\Tests\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\TEAM_WORK\Tests\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5664"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17255" windowHeight="5660" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="RegistrationUser" sheetId="1" r:id="rId1"/>
+    <sheet name="LoginUser" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
   <si>
     <t>TestName</t>
   </si>
@@ -57,12 +58,21 @@
   </si>
   <si>
     <t>ivan4o</t>
+  </si>
+  <si>
+    <t>LoginWithoutEmail</t>
+  </si>
+  <si>
+    <t>LoginWithPassword</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -92,9 +102,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -411,11 +427,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="43.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
@@ -479,4 +495,57 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="27.77734375" customWidth="1"/>
+    <col min="2" max="2" width="14.5546875" customWidth="1"/>
+    <col min="3" max="3" width="15.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1234</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added one more  Login test
</commit_message>
<xml_diff>
--- a/Tests/Data/DataSource.xlsx
+++ b/Tests/Data/DataSource.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
   <si>
     <t>TestName</t>
   </si>
@@ -63,10 +63,16 @@
     <t>LoginWithoutEmail</t>
   </si>
   <si>
-    <t>LoginWithPassword</t>
-  </si>
-  <si>
     <t>test</t>
+  </si>
+  <si>
+    <t>LoginWithIncorrectEmail</t>
+  </si>
+  <si>
+    <t>LoginWithoutPassword</t>
+  </si>
+  <si>
+    <t>test@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -499,16 +505,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="27.77734375" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" customWidth="1"/>
     <col min="3" max="3" width="15.109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -536,16 +542,25 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="C3" s="2">
         <v>1234</v>
       </c>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added one more RegistrationTest
</commit_message>
<xml_diff>
--- a/Tests/Data/DataSource.xlsx
+++ b/Tests/Data/DataSource.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17255" windowHeight="5660" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17255" windowHeight="5660"/>
   </bookViews>
   <sheets>
     <sheet name="RegistrationUser" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
   <si>
     <t>TestName</t>
   </si>
@@ -73,6 +73,15 @@
   </si>
   <si>
     <t>test@gmail.com</t>
+  </si>
+  <si>
+    <t>RegistrationWithoutPassword</t>
+  </si>
+  <si>
+    <t>IvanIvanov</t>
+  </si>
+  <si>
+    <t>email@abv.bg</t>
   </si>
 </sst>
 </file>
@@ -431,18 +440,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="43.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" customWidth="1"/>
     <col min="5" max="5" width="15.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -495,6 +504,17 @@
       </c>
       <c r="E3" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -507,8 +527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Update OleDb connection string
</commit_message>
<xml_diff>
--- a/Tests/Data/DataSource.xlsx
+++ b/Tests/Data/DataSource.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17830"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\TEAM_WORK\Tests\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\GitHub\QA-Automation-Teamwork\Tests\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17255" windowHeight="5660" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5664" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="RegistrationUser" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
   <si>
     <t>TestName</t>
   </si>
@@ -84,19 +84,16 @@
     <t>email@abv.bg</t>
   </si>
   <si>
-    <t>SuccessfulLogIn</t>
-  </si>
-  <si>
-    <t>georgi_vatashki@abv.bg</t>
-  </si>
-  <si>
-    <t>softuni123</t>
+    <t>admin@admin.com</t>
+  </si>
+  <si>
+    <t>LoginAsAdmin</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -455,7 +452,7 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="43.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.33203125" customWidth="1"/>
@@ -537,10 +534,10 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="27.77734375" customWidth="1"/>
     <col min="2" max="2" width="21.77734375" customWidth="1"/>
@@ -560,21 +557,21 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>9</v>
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
       </c>
       <c r="C2" s="2">
-        <v>1234</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C3" s="2">
         <v>1234</v>
@@ -582,21 +579,21 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" t="s">
-        <v>15</v>
+        <v>13</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1234</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added one more Registration test
</commit_message>
<xml_diff>
--- a/Tests/Data/DataSource.xlsx
+++ b/Tests/Data/DataSource.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\TEAM_WORK_REV_A\Tests\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\TEAM_WORK\Tests\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17255" windowHeight="5660" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17255" windowHeight="5660"/>
   </bookViews>
   <sheets>
     <sheet name="RegistrationUser" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
   <si>
     <t>TestName</t>
   </si>
@@ -94,6 +94,18 @@
   </si>
   <si>
     <t>a</t>
+  </si>
+  <si>
+    <t>RegistrationWithDifferentPasswords</t>
+  </si>
+  <si>
+    <t>softuni</t>
+  </si>
+  <si>
+    <t>qa</t>
+  </si>
+  <si>
+    <t>qa123</t>
   </si>
 </sst>
 </file>
@@ -452,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -529,6 +541,23 @@
         <v>17</v>
       </c>
     </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -539,7 +568,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
One more Registration Test
</commit_message>
<xml_diff>
--- a/Tests/Data/DataSource.xlsx
+++ b/Tests/Data/DataSource.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
   <si>
     <t>TestName</t>
   </si>
@@ -106,6 +106,9 @@
   </si>
   <si>
     <t>qa123</t>
+  </si>
+  <si>
+    <t>RegistrationWithoutFullName</t>
   </si>
 </sst>
 </file>
@@ -464,7 +467,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
@@ -556,6 +559,20 @@
       </c>
       <c r="E5" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6">
+        <v>123</v>
+      </c>
+      <c r="E6">
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Test register new user
</commit_message>
<xml_diff>
--- a/Tests/Data/DataSource.xlsx
+++ b/Tests/Data/DataSource.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17927"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\TEAM_WORK\Tests\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\GitHub\QA-Automation-Teamwork\Tests\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17255" windowHeight="5660"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5664"/>
   </bookViews>
   <sheets>
     <sheet name="RegistrationUser" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="34">
   <si>
     <t>TestName</t>
   </si>
@@ -109,12 +109,30 @@
   </si>
   <si>
     <t>RegistrationWithoutFullName</t>
+  </si>
+  <si>
+    <t>LoginAsUser</t>
+  </si>
+  <si>
+    <t>petkova.antoaneta@gmail.com</t>
+  </si>
+  <si>
+    <t>RegisterUser</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>name@example.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -144,7 +162,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -153,6 +171,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -467,16 +486,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="43.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" customWidth="1"/>
+    <col min="2" max="2" width="18.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.5546875" customWidth="1"/>
     <col min="4" max="4" width="15.6640625" customWidth="1"/>
     <col min="5" max="5" width="15.44140625" bestFit="1" customWidth="1"/>
@@ -500,28 +519,28 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
+      <c r="A2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
@@ -535,43 +554,60 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
         <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
         <v>18</v>
       </c>
-      <c r="D6">
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7">
         <v>123</v>
       </c>
-      <c r="E6">
+      <c r="E7">
         <v>123</v>
       </c>
     </row>
@@ -583,16 +619,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="27.77734375" customWidth="1"/>
-    <col min="2" max="2" width="21.77734375" customWidth="1"/>
+    <col min="2" max="2" width="27.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -620,21 +656,21 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>9</v>
+        <v>28</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>29</v>
       </c>
       <c r="C3" s="2">
-        <v>1234</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C4" s="2">
         <v>1234</v>
@@ -642,20 +678,31 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
+        <v>13</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1234</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>19</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added a new Login with created article test
</commit_message>
<xml_diff>
--- a/Tests/Data/DataSource.xlsx
+++ b/Tests/Data/DataSource.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17927"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\GitHub\QA-Automation-Teamwork\Tests\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\TEAM_WORK\Tests\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5664"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17255" windowHeight="5660" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="RegistrationUser" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="39">
   <si>
     <t>TestName</t>
   </si>
@@ -127,12 +127,27 @@
   </si>
   <si>
     <t>name@example.com</t>
+  </si>
+  <si>
+    <t>LoginWithCreatedArticle</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Blackcurrant</t>
+  </si>
+  <si>
+    <t>Content</t>
+  </si>
+  <si>
+    <t>Team</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -162,7 +177,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -172,6 +187,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -488,11 +509,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="43.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.5546875" bestFit="1" customWidth="1"/>
@@ -619,20 +640,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="27.77734375" customWidth="1"/>
     <col min="2" max="2" width="27.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.109375" customWidth="1"/>
+    <col min="4" max="4" width="12.77734375" customWidth="1"/>
+    <col min="5" max="5" width="15.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -642,31 +665,37 @@
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="D1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C2" s="2">
         <v>123</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>29</v>
       </c>
       <c r="C3" s="2">
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -676,8 +705,8 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
         <v>13</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -687,23 +716,40 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="2" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="2">
+        <v>123</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Create ArticleListPage and some tests
</commit_message>
<xml_diff>
--- a/Tests/Data/DataSource.xlsx
+++ b/Tests/Data/DataSource.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17927"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\TEAM_WORK\Tests\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\GitHub\QA-Automation-Teamwork\Tests\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17255" windowHeight="5660" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5664"/>
   </bookViews>
   <sheets>
     <sheet name="RegistrationUser" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="35">
   <si>
     <t>TestName</t>
   </si>
@@ -130,24 +130,12 @@
   </si>
   <si>
     <t>LoginWithCreatedArticle</t>
-  </si>
-  <si>
-    <t>Title</t>
-  </si>
-  <si>
-    <t>Blackcurrant</t>
-  </si>
-  <si>
-    <t>Content</t>
-  </si>
-  <si>
-    <t>Team</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -509,11 +497,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="43.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.5546875" bestFit="1" customWidth="1"/>
@@ -640,22 +628,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="27.77734375" customWidth="1"/>
     <col min="2" max="2" width="27.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.109375" customWidth="1"/>
-    <col min="4" max="4" width="12.77734375" customWidth="1"/>
-    <col min="5" max="5" width="15.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -665,14 +651,8 @@
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>20</v>
       </c>
@@ -683,7 +663,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>28</v>
       </c>
@@ -694,7 +674,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>11</v>
       </c>
@@ -705,7 +685,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>13</v>
       </c>
@@ -716,7 +696,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>14</v>
       </c>
@@ -724,7 +704,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>21</v>
       </c>
@@ -735,7 +715,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>34</v>
       </c>
@@ -744,12 +724,6 @@
       </c>
       <c r="C8" s="2">
         <v>123</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>